<commit_message>
fix(scoring): update PSS labels to match Excel format
- Changed 'Kode 1 Stres Ringan' → 'Stress Ringan'
- Changed 'Kode 2 Stres Sedang' → 'Stress Sedang'
- Changed 'Kode 3 Stres Berat' → 'Stress Berat'
- Updated validation script
- Validation result: PSS 18/18 (100%), SRQ 18/18 (100%)
</commit_message>
<xml_diff>
--- a/data_train.xlsx
+++ b/data_train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macos/Documents/UNIV/SM5/Asisya/asisya-web-pipe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9786252E-FD55-3848-A385-61283052E0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1989DA61-009B-A84D-BBCA-92C003FEC273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2500" windowWidth="26440" windowHeight="14420" activeTab="2" xr2:uid="{775AA019-D1A2-FA4A-8DA1-EFD9B9603518}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SRQ" sheetId="2" r:id="rId2"/>
     <sheet name="PSS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="26">
   <si>
     <t>Adelia Sekarsari</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Tidak Normal. Terdapat gejala psikologis seperti cemas dan depresi. Namun tidak terdapat penggunaan zat psikoaktif/narkoba, gejala episode psikotik dan gejala PTSD/gejala stress setelah trauma</t>
+  </si>
+  <si>
+    <t>Stress Ringan</t>
+  </si>
+  <si>
+    <t>Stress Sedang</t>
   </si>
 </sst>
 </file>
@@ -2889,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EF8738-5CCB-E145-A74E-27A3789A3A41}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2955,77 +2961,59 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="str">
-        <f t="shared" ref="A2:R2" si="0">IF(A1&gt;26,"Stress Berat",IF(A1&gt;13,"Stress Sedang","Stress Ringan"))</f>
-        <v>Stress Berat</v>
-      </c>
-      <c r="B2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="C2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="D2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="E2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="F2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="G2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="H2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="I2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="J2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="K2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="L2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="M2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="N2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="O2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="P2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="Q2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
-      </c>
-      <c r="R2" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Stress Berat</v>
+      <c r="A2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>